<commit_message>
Adjust temperature data and nutrition
</commit_message>
<xml_diff>
--- a/src/datagen/resources/data/frostedheart/data/biome_temperature.xlsx
+++ b/src/datagen/resources/data/frostedheart/data/biome_temperature.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyc/Development/FrostedHeart/src/datagen/resources/data/frostedheart/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56CD73B-8CF5-5F44-B745-6B9C70C5E51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="biome_temperature" sheetId="1" r:id="rId3"/>
+    <sheet name="biome_temperature" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
-  <si>
-    <t/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>biome</t>
   </si>
@@ -112,33 +116,36 @@
   </si>
   <si>
     <t>terralith:gravel_desert</t>
+  </si>
+  <si>
+    <t>terralith:cave/underground_jungle</t>
+  </si>
+  <si>
+    <t>terralith:cave/thermal_caves</t>
+  </si>
+  <si>
+    <t>terralith:cave/infested_caves</t>
+  </si>
+  <si>
+    <t>terralith:cave/mantle_caves</t>
+  </si>
+  <si>
+    <t>the_winter_rescue:magmatic_deposits</t>
+  </si>
+  <si>
+    <t>the_winter_rescue:hydrothermal_deposits</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="等线"/>
-      <charset val="134"/>
-      <color rgb="FF175CEB"/>
-      <sz val="10"/>
-      <u/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Segoe UI Symbol"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -155,23 +162,28 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -293,7 +305,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -317,9 +329,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -343,7 +355,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -378,7 +390,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -396,7 +408,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -421,51 +433,49 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}"/>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr/>
-  <dimension ref="C31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView showGridLines="true" tabSelected="true" topLeftCell="A7" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="243" zoomScaleNormal="243" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="47.75" customWidth="true"/>
-    <col min="2" max="2" width="13.625" customWidth="true"/>
+    <col min="1" max="1" width="47.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="15.25" customHeight="1">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.3975" customHeight="true">
-      <c r="A2" t="s">
-        <v>3</v>
       </c>
       <c r="B2">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.3975" customHeight="true">
+    <row r="3" spans="1:2" ht="15.25" customHeight="1">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -473,7 +483,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>-2</v>
@@ -481,7 +491,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>-3</v>
@@ -489,7 +499,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -497,7 +507,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>-3</v>
@@ -505,7 +515,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>-30</v>
@@ -513,7 +523,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>-3</v>
@@ -521,7 +531,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>-2</v>
@@ -529,7 +539,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>-2</v>
@@ -537,7 +547,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>-2</v>
@@ -545,7 +555,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -553,7 +563,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -561,7 +571,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>5</v>
@@ -569,7 +579,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -577,7 +587,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -585,7 +595,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>5</v>
@@ -593,7 +603,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -601,7 +611,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -609,7 +619,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -617,7 +627,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -625,7 +635,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -633,7 +643,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -641,7 +651,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -649,7 +659,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -657,7 +667,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -665,7 +675,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -673,7 +683,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -681,7 +691,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30">
         <v>-10</v>
@@ -689,13 +699,62 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31">
         <v>-1</v>
       </c>
     </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B31"/>
+  <autoFilter ref="A1:B31" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix lush caves temp
</commit_message>
<xml_diff>
--- a/src/datagen/resources/data/frostedheart/data/biome_temperature.xlsx
+++ b/src/datagen/resources/data/frostedheart/data/biome_temperature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyc/Development/FrostedHeart/src/datagen/resources/data/frostedheart/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56CD73B-8CF5-5F44-B745-6B9C70C5E51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F94B0E-4ED4-2743-A841-C6577017B564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="biome_temperature" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>biome</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>the_winter_rescue:hydrothermal_deposits</t>
+  </si>
+  <si>
+    <t>minecraft:lush_caves</t>
   </si>
 </sst>
 </file>
@@ -445,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="243" zoomScaleNormal="243" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="243" zoomScaleNormal="243" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -753,6 +756,14 @@
         <v>40</v>
       </c>
     </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B31" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>